<commit_message>
Final push for real
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27C613EB-2548-4302-814D-E5FC81229185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E2E98A-A348-4F15-9F6C-646A93BCE607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="-21710" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>Create a Project Schedule in this worksheet.
 Enter title of this project in cell B1. 
@@ -108,10 +108,6 @@
   </si>
   <si>
     <t>TASK</t>
-  </si>
-  <si>
-    <t>ASSIGNED
-TO</t>
   </si>
   <si>
     <t>PROGRESS</t>
@@ -189,9 +185,6 @@
     <t>Task 8</t>
   </si>
   <si>
-    <t>Landlord page</t>
-  </si>
-  <si>
     <t>Task 9</t>
   </si>
   <si>
@@ -205,9 +198,6 @@
   </si>
   <si>
     <t>Task 11</t>
-  </si>
-  <si>
-    <t>Adding database</t>
   </si>
   <si>
     <t>Sample phase title block</t>
@@ -299,19 +289,34 @@
   <si>
     <t>Businesses will find invoices, time sheets, inventory trackers, financial statements, and project planning templates. Teachers and students will find resources such as class schedules, grade books, and attendance sheets. Organize your family life with meal planners, checklists, and exercise logs. Each template is thoroughly researched, refined, and improved over time through feedback from thousands of users.</t>
   </si>
+  <si>
+    <t>Adding saving functionalities</t>
+  </si>
+  <si>
+    <t>Description of Task</t>
+  </si>
+  <si>
+    <t>Task 15</t>
+  </si>
+  <si>
+    <t>Task 16</t>
+  </si>
+  <si>
+    <t>Bug fixes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="166" formatCode="ddd\,\ m/d/yyyy"/>
-    <numFmt numFmtId="167" formatCode="mmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="168" formatCode="d"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
+    <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="d"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,7 +667,7 @@
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -671,10 +676,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" applyFill="0">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" applyFill="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyFill="0">
@@ -711,13 +716,13 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -737,10 +742,10 @@
     <xf numFmtId="9" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,15 +816,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -829,7 +825,7 @@
     <xf numFmtId="9" fontId="5" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="6" borderId="2" xfId="10" applyFill="1">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="12" applyFill="1">
@@ -844,28 +840,37 @@
     <xf numFmtId="9" fontId="5" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="7" borderId="2" xfId="10" applyFill="1">
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1526,25 +1531,25 @@
   </sheetPr>
   <dimension ref="A1:BS35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M30" sqref="M30"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="37" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="71" width="2.5703125" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="37" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="71" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" ht="30" customHeight="1">
+    <row r="1" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -1558,14 +1563,14 @@
       <c r="H1" s="2"/>
       <c r="I1" s="45"/>
     </row>
-    <row r="2" spans="1:71" ht="30" customHeight="1">
+    <row r="2" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="42"/>
       <c r="I2" s="46"/>
     </row>
-    <row r="3" spans="1:71" ht="30" customHeight="1">
+    <row r="3" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
         <v>3</v>
       </c>
@@ -1575,12 +1580,12 @@
       </c>
       <c r="D3" s="65"/>
       <c r="E3" s="66">
-        <f ca="1">TODAY()-3</f>
-        <v>44670</v>
+        <f>DATE(2022, 4, 20)</f>
+        <v>44671</v>
       </c>
       <c r="F3" s="66"/>
     </row>
-    <row r="4" spans="1:71" ht="30" customHeight="1">
+    <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
@@ -1591,89 +1596,89 @@
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="48" t="s">
+      <c r="I4" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="48" t="s">
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="50"/>
-      <c r="W4" s="48" t="s">
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="62"/>
+      <c r="U4" s="62"/>
+      <c r="V4" s="63"/>
+      <c r="W4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="X4" s="49"/>
-      <c r="Y4" s="49"/>
-      <c r="Z4" s="49"/>
-      <c r="AA4" s="49"/>
-      <c r="AB4" s="49"/>
-      <c r="AC4" s="50"/>
-      <c r="AD4" s="48" t="s">
+      <c r="X4" s="62"/>
+      <c r="Y4" s="62"/>
+      <c r="Z4" s="62"/>
+      <c r="AA4" s="62"/>
+      <c r="AB4" s="62"/>
+      <c r="AC4" s="63"/>
+      <c r="AD4" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="AE4" s="49"/>
-      <c r="AF4" s="49"/>
-      <c r="AG4" s="49"/>
-      <c r="AH4" s="49"/>
-      <c r="AI4" s="49"/>
-      <c r="AJ4" s="50"/>
-      <c r="AK4" s="48" t="s">
+      <c r="AE4" s="62"/>
+      <c r="AF4" s="62"/>
+      <c r="AG4" s="62"/>
+      <c r="AH4" s="62"/>
+      <c r="AI4" s="62"/>
+      <c r="AJ4" s="63"/>
+      <c r="AK4" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="AL4" s="49"/>
-      <c r="AM4" s="49"/>
-      <c r="AN4" s="49"/>
-      <c r="AO4" s="49"/>
-      <c r="AP4" s="49"/>
-      <c r="AQ4" s="50"/>
-      <c r="AR4" s="48" t="s">
+      <c r="AL4" s="62"/>
+      <c r="AM4" s="62"/>
+      <c r="AN4" s="62"/>
+      <c r="AO4" s="62"/>
+      <c r="AP4" s="62"/>
+      <c r="AQ4" s="63"/>
+      <c r="AR4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AS4" s="49"/>
-      <c r="AT4" s="49"/>
-      <c r="AU4" s="49"/>
-      <c r="AV4" s="49"/>
-      <c r="AW4" s="49"/>
-      <c r="AX4" s="50"/>
-      <c r="AY4" s="48" t="s">
+      <c r="AS4" s="62"/>
+      <c r="AT4" s="62"/>
+      <c r="AU4" s="62"/>
+      <c r="AV4" s="62"/>
+      <c r="AW4" s="62"/>
+      <c r="AX4" s="63"/>
+      <c r="AY4" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="AZ4" s="49"/>
-      <c r="BA4" s="49"/>
-      <c r="BB4" s="49"/>
-      <c r="BC4" s="49"/>
-      <c r="BD4" s="49"/>
-      <c r="BE4" s="50"/>
-      <c r="BF4" s="48" t="s">
+      <c r="AZ4" s="62"/>
+      <c r="BA4" s="62"/>
+      <c r="BB4" s="62"/>
+      <c r="BC4" s="62"/>
+      <c r="BD4" s="62"/>
+      <c r="BE4" s="63"/>
+      <c r="BF4" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="BG4" s="49"/>
-      <c r="BH4" s="49"/>
-      <c r="BI4" s="49"/>
-      <c r="BJ4" s="49"/>
-      <c r="BK4" s="49"/>
-      <c r="BL4" s="50"/>
-      <c r="BM4" s="48" t="s">
+      <c r="BG4" s="62"/>
+      <c r="BH4" s="62"/>
+      <c r="BI4" s="62"/>
+      <c r="BJ4" s="62"/>
+      <c r="BK4" s="62"/>
+      <c r="BL4" s="63"/>
+      <c r="BM4" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="BN4" s="49"/>
-      <c r="BO4" s="49"/>
-      <c r="BP4" s="49"/>
-      <c r="BQ4" s="49"/>
-      <c r="BR4" s="49"/>
-      <c r="BS4" s="50"/>
-    </row>
-    <row r="5" spans="1:71" ht="15" customHeight="1">
+      <c r="BN4" s="62"/>
+      <c r="BO4" s="62"/>
+      <c r="BP4" s="62"/>
+      <c r="BQ4" s="62"/>
+      <c r="BR4" s="62"/>
+      <c r="BS4" s="63"/>
+    </row>
+    <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="38" t="s">
         <v>16</v>
       </c>
@@ -1684,259 +1689,259 @@
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
       <c r="I5" s="11">
-        <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
+        <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44669</v>
       </c>
       <c r="J5" s="10">
-        <f ca="1">I5+1</f>
+        <f>I5+1</f>
         <v>44670</v>
       </c>
       <c r="K5" s="10">
-        <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
+        <f>J5+1</f>
         <v>44671</v>
       </c>
       <c r="L5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="K5:AX5" si="0">K5+1</f>
         <v>44672</v>
       </c>
       <c r="M5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f>L5+1</f>
         <v>44673</v>
       </c>
       <c r="N5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44674</v>
       </c>
       <c r="O5" s="12">
-        <f ca="1">N5+1</f>
+        <f>N5+1</f>
         <v>44675</v>
       </c>
       <c r="P5" s="11">
-        <f ca="1">O5+1</f>
+        <f>O5+1</f>
         <v>44676</v>
       </c>
       <c r="Q5" s="10">
-        <f ca="1">P5+1</f>
+        <f>P5+1</f>
         <v>44677</v>
       </c>
       <c r="R5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44678</v>
       </c>
       <c r="S5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44679</v>
       </c>
       <c r="T5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44680</v>
       </c>
       <c r="U5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44681</v>
       </c>
       <c r="V5" s="12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44682</v>
       </c>
       <c r="W5" s="11">
-        <f ca="1">V5+1</f>
+        <f>V5+1</f>
         <v>44683</v>
       </c>
       <c r="X5" s="10">
-        <f ca="1">W5+1</f>
+        <f>W5+1</f>
         <v>44684</v>
       </c>
       <c r="Y5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44685</v>
       </c>
       <c r="Z5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44686</v>
       </c>
       <c r="AA5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44687</v>
       </c>
       <c r="AB5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44688</v>
       </c>
       <c r="AC5" s="12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44689</v>
       </c>
       <c r="AD5" s="11">
-        <f ca="1">AC5+1</f>
+        <f>AC5+1</f>
         <v>44690</v>
       </c>
       <c r="AE5" s="10">
-        <f ca="1">AD5+1</f>
+        <f>AD5+1</f>
         <v>44691</v>
       </c>
       <c r="AF5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44692</v>
       </c>
       <c r="AG5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44693</v>
       </c>
       <c r="AH5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44694</v>
       </c>
       <c r="AI5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44695</v>
       </c>
       <c r="AJ5" s="12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44696</v>
       </c>
       <c r="AK5" s="11">
-        <f ca="1">AJ5+1</f>
+        <f>AJ5+1</f>
         <v>44697</v>
       </c>
       <c r="AL5" s="10">
-        <f ca="1">AK5+1</f>
+        <f>AK5+1</f>
         <v>44698</v>
       </c>
       <c r="AM5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44699</v>
       </c>
       <c r="AN5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44700</v>
       </c>
       <c r="AO5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44701</v>
       </c>
       <c r="AP5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44702</v>
       </c>
       <c r="AQ5" s="12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44703</v>
       </c>
       <c r="AR5" s="11">
-        <f ca="1">AQ5+1</f>
+        <f>AQ5+1</f>
         <v>44704</v>
       </c>
       <c r="AS5" s="10">
-        <f ca="1">AR5+1</f>
+        <f>AR5+1</f>
         <v>44705</v>
       </c>
       <c r="AT5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44706</v>
       </c>
       <c r="AU5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44707</v>
       </c>
       <c r="AV5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44708</v>
       </c>
       <c r="AW5" s="10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44709</v>
       </c>
       <c r="AX5" s="12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44710</v>
       </c>
       <c r="AY5" s="11">
-        <f ca="1">AX5+1</f>
+        <f>AX5+1</f>
         <v>44711</v>
       </c>
       <c r="AZ5" s="10">
-        <f ca="1">AY5+1</f>
+        <f>AY5+1</f>
         <v>44712</v>
       </c>
       <c r="BA5" s="10">
-        <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
+        <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
         <v>44713</v>
       </c>
       <c r="BB5" s="10">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>44714</v>
       </c>
       <c r="BC5" s="10">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>44715</v>
       </c>
       <c r="BD5" s="10">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>44716</v>
       </c>
       <c r="BE5" s="12">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>44717</v>
       </c>
       <c r="BF5" s="11">
-        <f ca="1">BE5+1</f>
+        <f>BE5+1</f>
         <v>44718</v>
       </c>
       <c r="BG5" s="10">
-        <f ca="1">BF5+1</f>
+        <f>BF5+1</f>
         <v>44719</v>
       </c>
       <c r="BH5" s="10">
-        <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
+        <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
         <v>44720</v>
       </c>
       <c r="BI5" s="10">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>44721</v>
       </c>
       <c r="BJ5" s="10">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>44722</v>
       </c>
       <c r="BK5" s="10">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>44723</v>
       </c>
       <c r="BL5" s="12">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>44724</v>
       </c>
       <c r="BM5" s="11">
-        <f ca="1">BL5+1</f>
+        <f>BL5+1</f>
         <v>44725</v>
       </c>
       <c r="BN5" s="10">
-        <f ca="1">BM5+1</f>
+        <f>BM5+1</f>
         <v>44726</v>
       </c>
       <c r="BO5" s="10">
-        <f t="shared" ref="BO5" ca="1" si="3">BN5+1</f>
+        <f t="shared" ref="BO5" si="3">BN5+1</f>
         <v>44727</v>
       </c>
       <c r="BP5" s="10">
-        <f t="shared" ref="BP5" ca="1" si="4">BO5+1</f>
+        <f t="shared" ref="BP5" si="4">BO5+1</f>
         <v>44728</v>
       </c>
       <c r="BQ5" s="10">
-        <f t="shared" ref="BQ5" ca="1" si="5">BP5+1</f>
+        <f t="shared" ref="BQ5" si="5">BP5+1</f>
         <v>44729</v>
       </c>
       <c r="BR5" s="10">
-        <f t="shared" ref="BR5" ca="1" si="6">BQ5+1</f>
+        <f t="shared" ref="BR5" si="6">BQ5+1</f>
         <v>44730</v>
       </c>
       <c r="BS5" s="12">
-        <f t="shared" ref="BS5" ca="1" si="7">BR5+1</f>
+        <f t="shared" ref="BS5" si="7">BR5+1</f>
         <v>44731</v>
       </c>
     </row>
-    <row r="6" spans="1:71" ht="30" customHeight="1">
+    <row r="6" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>17</v>
       </c>
@@ -1944,282 +1949,282 @@
         <v>18</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>22</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="13" t="str">
+        <f t="shared" ref="I6" si="8">LEFT(TEXT(I5,"ddd"),1)</f>
+        <v>M</v>
+      </c>
+      <c r="J6" s="13" t="str">
+        <f t="shared" ref="J6:AR6" si="9">LEFT(TEXT(J5,"ddd"),1)</f>
+        <v>T</v>
+      </c>
+      <c r="K6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>W</v>
+      </c>
+      <c r="L6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>T</v>
+      </c>
+      <c r="M6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>F</v>
+      </c>
+      <c r="N6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="O6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="P6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>M</v>
+      </c>
+      <c r="Q6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>T</v>
+      </c>
+      <c r="R6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>W</v>
+      </c>
+      <c r="S6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>T</v>
+      </c>
+      <c r="T6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>F</v>
+      </c>
+      <c r="U6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="V6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="W6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>M</v>
+      </c>
+      <c r="X6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>T</v>
+      </c>
+      <c r="Y6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>W</v>
+      </c>
+      <c r="Z6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>T</v>
+      </c>
+      <c r="AA6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>F</v>
+      </c>
+      <c r="AB6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="AC6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="AD6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>M</v>
+      </c>
+      <c r="AE6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>T</v>
+      </c>
+      <c r="AF6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>W</v>
+      </c>
+      <c r="AG6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>T</v>
+      </c>
+      <c r="AH6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>F</v>
+      </c>
+      <c r="AI6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="AJ6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="AK6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>M</v>
+      </c>
+      <c r="AL6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>T</v>
+      </c>
+      <c r="AM6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>W</v>
+      </c>
+      <c r="AN6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>T</v>
+      </c>
+      <c r="AO6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>F</v>
+      </c>
+      <c r="AP6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="AQ6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="AR6" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>M</v>
+      </c>
+      <c r="AS6" s="13" t="str">
+        <f t="shared" ref="AS6:BL6" si="10">LEFT(TEXT(AS5,"ddd"),1)</f>
+        <v>T</v>
+      </c>
+      <c r="AT6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>W</v>
+      </c>
+      <c r="AU6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>T</v>
+      </c>
+      <c r="AV6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>F</v>
+      </c>
+      <c r="AW6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>S</v>
+      </c>
+      <c r="AX6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>S</v>
+      </c>
+      <c r="AY6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>M</v>
+      </c>
+      <c r="AZ6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>T</v>
+      </c>
+      <c r="BA6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>W</v>
+      </c>
+      <c r="BB6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>T</v>
+      </c>
+      <c r="BC6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>F</v>
+      </c>
+      <c r="BD6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>S</v>
+      </c>
+      <c r="BE6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>S</v>
+      </c>
+      <c r="BF6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>M</v>
+      </c>
+      <c r="BG6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>T</v>
+      </c>
+      <c r="BH6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>W</v>
+      </c>
+      <c r="BI6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>T</v>
+      </c>
+      <c r="BJ6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>F</v>
+      </c>
+      <c r="BK6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>S</v>
+      </c>
+      <c r="BL6" s="13" t="str">
+        <f t="shared" si="10"/>
+        <v>S</v>
+      </c>
+      <c r="BM6" s="13" t="str">
+        <f t="shared" ref="BM6:BS6" si="11">LEFT(TEXT(BM5,"ddd"),1)</f>
+        <v>M</v>
+      </c>
+      <c r="BN6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>T</v>
+      </c>
+      <c r="BO6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>W</v>
+      </c>
+      <c r="BP6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>T</v>
+      </c>
+      <c r="BQ6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>F</v>
+      </c>
+      <c r="BR6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>S</v>
+      </c>
+      <c r="BS6" s="13" t="str">
+        <f t="shared" si="11"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="7" spans="1:71" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
         <v>23</v>
-      </c>
-      <c r="I6" s="13" t="str">
-        <f t="shared" ref="I6" ca="1" si="8">LEFT(TEXT(I5,"ddd"),1)</f>
-        <v>п</v>
-      </c>
-      <c r="J6" s="13" t="str">
-        <f t="shared" ref="J6:AR6" ca="1" si="9">LEFT(TEXT(J5,"ddd"),1)</f>
-        <v>в</v>
-      </c>
-      <c r="K6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>с</v>
-      </c>
-      <c r="L6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>ч</v>
-      </c>
-      <c r="M6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>п</v>
-      </c>
-      <c r="N6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>с</v>
-      </c>
-      <c r="O6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>н</v>
-      </c>
-      <c r="P6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>п</v>
-      </c>
-      <c r="Q6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>в</v>
-      </c>
-      <c r="R6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>с</v>
-      </c>
-      <c r="S6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>ч</v>
-      </c>
-      <c r="T6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>п</v>
-      </c>
-      <c r="U6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>с</v>
-      </c>
-      <c r="V6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>н</v>
-      </c>
-      <c r="W6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>п</v>
-      </c>
-      <c r="X6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>в</v>
-      </c>
-      <c r="Y6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>с</v>
-      </c>
-      <c r="Z6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>ч</v>
-      </c>
-      <c r="AA6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>п</v>
-      </c>
-      <c r="AB6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>с</v>
-      </c>
-      <c r="AC6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>н</v>
-      </c>
-      <c r="AD6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>п</v>
-      </c>
-      <c r="AE6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>в</v>
-      </c>
-      <c r="AF6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>с</v>
-      </c>
-      <c r="AG6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>ч</v>
-      </c>
-      <c r="AH6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>п</v>
-      </c>
-      <c r="AI6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>с</v>
-      </c>
-      <c r="AJ6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>н</v>
-      </c>
-      <c r="AK6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>п</v>
-      </c>
-      <c r="AL6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>в</v>
-      </c>
-      <c r="AM6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>с</v>
-      </c>
-      <c r="AN6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>ч</v>
-      </c>
-      <c r="AO6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>п</v>
-      </c>
-      <c r="AP6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>с</v>
-      </c>
-      <c r="AQ6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>н</v>
-      </c>
-      <c r="AR6" s="13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>п</v>
-      </c>
-      <c r="AS6" s="13" t="str">
-        <f t="shared" ref="AS6:BL6" ca="1" si="10">LEFT(TEXT(AS5,"ddd"),1)</f>
-        <v>в</v>
-      </c>
-      <c r="AT6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>с</v>
-      </c>
-      <c r="AU6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>ч</v>
-      </c>
-      <c r="AV6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>п</v>
-      </c>
-      <c r="AW6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>с</v>
-      </c>
-      <c r="AX6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>н</v>
-      </c>
-      <c r="AY6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>п</v>
-      </c>
-      <c r="AZ6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>в</v>
-      </c>
-      <c r="BA6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>с</v>
-      </c>
-      <c r="BB6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>ч</v>
-      </c>
-      <c r="BC6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>п</v>
-      </c>
-      <c r="BD6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>с</v>
-      </c>
-      <c r="BE6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>н</v>
-      </c>
-      <c r="BF6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>п</v>
-      </c>
-      <c r="BG6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>в</v>
-      </c>
-      <c r="BH6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>с</v>
-      </c>
-      <c r="BI6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>ч</v>
-      </c>
-      <c r="BJ6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>п</v>
-      </c>
-      <c r="BK6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>с</v>
-      </c>
-      <c r="BL6" s="13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>н</v>
-      </c>
-      <c r="BM6" s="13" t="str">
-        <f t="shared" ref="BM6:BS6" ca="1" si="11">LEFT(TEXT(BM5,"ddd"),1)</f>
-        <v>п</v>
-      </c>
-      <c r="BN6" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>в</v>
-      </c>
-      <c r="BO6" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>с</v>
-      </c>
-      <c r="BP6" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>ч</v>
-      </c>
-      <c r="BQ6" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>п</v>
-      </c>
-      <c r="BR6" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>с</v>
-      </c>
-      <c r="BS6" s="13" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>н</v>
-      </c>
-    </row>
-    <row r="7" spans="1:71" ht="30" hidden="1" customHeight="1">
-      <c r="A7" s="37" t="s">
-        <v>24</v>
       </c>
       <c r="C7" s="40"/>
       <c r="E7"/>
       <c r="H7" t="str">
-        <f ca="1">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I7" s="23"/>
@@ -2286,35 +2291,35 @@
       <c r="BR7" s="23"/>
       <c r="BS7" s="23"/>
     </row>
-    <row r="8" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="8" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="C8" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="53">
+      <c r="D8" s="50">
         <v>1</v>
       </c>
-      <c r="E8" s="54">
-        <f ca="1">Project_Start</f>
-        <v>44670</v>
-      </c>
-      <c r="F8" s="54">
-        <f ca="1">E8</f>
-        <v>44670</v>
+      <c r="E8" s="51">
+        <f>Project_Start</f>
+        <v>44671</v>
+      </c>
+      <c r="F8" s="51">
+        <f>E8</f>
+        <v>44671</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16">
-        <f t="shared" ref="H8:H32" ca="1" si="12">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H32" si="12">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>1</v>
       </c>
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>
-      <c r="K8" s="51"/>
+      <c r="K8" s="48"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23"/>
       <c r="N8" s="23"/>
@@ -2376,30 +2381,30 @@
       <c r="BR8" s="23"/>
       <c r="BS8" s="23"/>
     </row>
-    <row r="9" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="9" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="C9" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="53">
+      <c r="D9" s="50">
         <v>1</v>
       </c>
-      <c r="E9" s="54">
-        <f ca="1">F8+1</f>
-        <v>44671</v>
-      </c>
-      <c r="F9" s="54">
-        <f ca="1">E9</f>
-        <v>44671</v>
+      <c r="E9" s="51">
+        <f>F8+1</f>
+        <v>44672</v>
+      </c>
+      <c r="F9" s="51">
+        <f>E9</f>
+        <v>44672</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="I9" s="23"/>
@@ -2466,29 +2471,29 @@
       <c r="BR9" s="23"/>
       <c r="BS9" s="23"/>
     </row>
-    <row r="10" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="10" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37"/>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="53">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="54">
-        <f ca="1">F9+1</f>
-        <v>44672</v>
-      </c>
-      <c r="F10" s="54">
-        <f ca="1">E10+5</f>
-        <v>44677</v>
+      <c r="D10" s="50">
+        <v>1</v>
+      </c>
+      <c r="E10" s="51">
+        <f>F9+1</f>
+        <v>44673</v>
+      </c>
+      <c r="F10" s="51">
+        <f>E10</f>
+        <v>44673</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16">
-        <f t="shared" ca="1" si="12"/>
-        <v>6</v>
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
@@ -2554,29 +2559,29 @@
       <c r="BR10" s="23"/>
       <c r="BS10" s="23"/>
     </row>
-    <row r="11" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="11" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37"/>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="53">
-        <v>0.75</v>
-      </c>
-      <c r="E11" s="54">
-        <f ca="1">F9+1</f>
-        <v>44672</v>
-      </c>
-      <c r="F11" s="54">
-        <f ca="1">E9+4</f>
-        <v>44675</v>
+      <c r="D11" s="50">
+        <v>1</v>
+      </c>
+      <c r="E11" s="51">
+        <f>F9+1</f>
+        <v>44673</v>
+      </c>
+      <c r="F11" s="51">
+        <f>E9+1</f>
+        <v>44673</v>
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="16">
-        <f t="shared" ca="1" si="12"/>
-        <v>4</v>
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="I11" s="23"/>
       <c r="J11" s="23"/>
@@ -2642,13 +2647,13 @@
       <c r="BR11" s="23"/>
       <c r="BS11" s="23"/>
     </row>
-    <row r="12" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="12" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="37"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
       <c r="I12" s="23"/>
@@ -2715,28 +2720,28 @@
       <c r="BR12" s="23"/>
       <c r="BS12" s="23"/>
     </row>
-    <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="38"/>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="53">
-        <v>0</v>
-      </c>
-      <c r="E13" s="54">
-        <f ca="1">E9+5</f>
+      <c r="D13" s="50">
+        <v>1</v>
+      </c>
+      <c r="E13" s="51">
+        <f>E9+4</f>
         <v>44676</v>
       </c>
-      <c r="F13" s="54">
-        <f ca="1">E13+4</f>
+      <c r="F13" s="51">
+        <f>E13+4</f>
         <v>44680</v>
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="16">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="I13" s="23"/>
@@ -2803,28 +2808,28 @@
       <c r="BR13" s="23"/>
       <c r="BS13" s="23"/>
     </row>
-    <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37"/>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="53">
-        <v>0</v>
-      </c>
-      <c r="E14" s="54">
-        <f ca="1">E13</f>
+      <c r="D14" s="50">
+        <v>1</v>
+      </c>
+      <c r="E14" s="51">
+        <f>E13</f>
         <v>44676</v>
       </c>
-      <c r="F14" s="54">
-        <f ca="1">E14+4</f>
+      <c r="F14" s="51">
+        <f>E14+4</f>
         <v>44680</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="I14" s="23"/>
@@ -2891,13 +2896,13 @@
       <c r="BR14" s="23"/>
       <c r="BS14" s="23"/>
     </row>
-    <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="23"/>
@@ -2964,29 +2969,29 @@
       <c r="BR15" s="23"/>
       <c r="BS15" s="23"/>
     </row>
-    <row r="16" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="16" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37"/>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="53">
-        <v>0</v>
-      </c>
-      <c r="E16" s="54">
-        <f ca="1">E8+13</f>
+      <c r="D16" s="50">
+        <v>1</v>
+      </c>
+      <c r="E16" s="51">
+        <f>E8+12</f>
         <v>44683</v>
       </c>
-      <c r="F16" s="54">
-        <f ca="1">E16+5</f>
-        <v>44688</v>
+      <c r="F16" s="51">
+        <f>E16+4</f>
+        <v>44687</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16">
-        <f t="shared" ca="1" si="12"/>
-        <v>6</v>
+        <f t="shared" si="12"/>
+        <v>5</v>
       </c>
       <c r="I16" s="23"/>
       <c r="J16" s="23"/>
@@ -3052,29 +3057,29 @@
       <c r="BR16" s="23"/>
       <c r="BS16" s="23"/>
     </row>
-    <row r="17" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="17" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37"/>
-      <c r="B17" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="53">
-        <v>0</v>
-      </c>
-      <c r="E17" s="54">
-        <f ca="1">E8+13</f>
+      <c r="B17" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="50">
+        <v>1</v>
+      </c>
+      <c r="E17" s="51">
+        <f>E8+12</f>
         <v>44683</v>
       </c>
-      <c r="F17" s="54">
-        <f ca="1">E16+6</f>
-        <v>44689</v>
+      <c r="F17" s="51">
+        <f>E16+4</f>
+        <v>44687</v>
       </c>
       <c r="G17" s="16"/>
       <c r="H17" s="16">
-        <f t="shared" ca="1" si="12"/>
-        <v>7</v>
+        <f t="shared" si="12"/>
+        <v>5</v>
       </c>
       <c r="I17" s="23"/>
       <c r="J17" s="23"/>
@@ -3140,13 +3145,13 @@
       <c r="BR17" s="23"/>
       <c r="BS17" s="23"/>
     </row>
-    <row r="18" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="18" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="37"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="23"/>
@@ -3213,28 +3218,28 @@
       <c r="BR18" s="23"/>
       <c r="BS18" s="23"/>
     </row>
-    <row r="19" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="19" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37"/>
-      <c r="B19" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="53">
-        <v>0</v>
-      </c>
-      <c r="E19" s="54">
-        <f ca="1">E17+7</f>
+      <c r="B19" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="50">
+        <v>1</v>
+      </c>
+      <c r="E19" s="51">
+        <f>E17+7</f>
         <v>44690</v>
       </c>
-      <c r="F19" s="54">
-        <f ca="1">E19+6</f>
+      <c r="F19" s="51">
+        <f>E19+6</f>
         <v>44696</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="16">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="I19" s="23"/>
@@ -3301,28 +3306,28 @@
       <c r="BR19" s="23"/>
       <c r="BS19" s="23"/>
     </row>
-    <row r="20" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="20" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37"/>
-      <c r="B20" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="53">
-        <v>0</v>
-      </c>
-      <c r="E20" s="54">
-        <f ca="1">E17+7</f>
+      <c r="B20" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="50">
+        <v>1</v>
+      </c>
+      <c r="E20" s="51">
+        <f>E17+7</f>
         <v>44690</v>
       </c>
-      <c r="F20" s="54">
-        <f ca="1">E20+6</f>
+      <c r="F20" s="51">
+        <f>E20+6</f>
         <v>44696</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="16">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="I20" s="23"/>
@@ -3389,13 +3394,13 @@
       <c r="BR20" s="23"/>
       <c r="BS20" s="23"/>
     </row>
-    <row r="21" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="21" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
       <c r="I21" s="23"/>
@@ -3462,29 +3467,29 @@
       <c r="BR21" s="23"/>
       <c r="BS21" s="23"/>
     </row>
-    <row r="22" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="22" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37"/>
-      <c r="B22" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="53">
-        <v>0</v>
-      </c>
-      <c r="E22" s="54">
-        <f ca="1">E20+7</f>
+      <c r="B22" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="50">
+        <v>1</v>
+      </c>
+      <c r="E22" s="51">
+        <f>E20+7</f>
         <v>44697</v>
       </c>
-      <c r="F22" s="54">
-        <f ca="1">E22+6</f>
-        <v>44703</v>
+      <c r="F22" s="51">
+        <f>E22+4</f>
+        <v>44701</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="16">
-        <f t="shared" ca="1" si="12"/>
-        <v>7</v>
+        <f t="shared" si="12"/>
+        <v>5</v>
       </c>
       <c r="I22" s="23"/>
       <c r="J22" s="23"/>
@@ -3550,20 +3555,20 @@
       <c r="BR22" s="23"/>
       <c r="BS22" s="23"/>
     </row>
-    <row r="23" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="62"/>
+        <v>46</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="59"/>
       <c r="G23" s="16"/>
       <c r="H23" s="16" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I23" s="23"/>
@@ -3630,29 +3635,29 @@
       <c r="BR23" s="23"/>
       <c r="BS23" s="23"/>
     </row>
-    <row r="24" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="24" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="37"/>
-      <c r="B24" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="53">
-        <v>0</v>
-      </c>
-      <c r="E24" s="54">
-        <f ca="1">E22+7</f>
+      <c r="B24" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="50">
+        <v>1</v>
+      </c>
+      <c r="E24" s="51">
+        <f>E22+7</f>
         <v>44704</v>
       </c>
-      <c r="F24" s="54">
-        <f ca="1">E24+6</f>
-        <v>44710</v>
+      <c r="F24" s="51">
+        <f>E24+4</f>
+        <v>44708</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="16">
-        <f t="shared" ca="1" si="12"/>
-        <v>7</v>
+        <f t="shared" si="12"/>
+        <v>5</v>
       </c>
       <c r="I24" s="23"/>
       <c r="J24" s="23"/>
@@ -3718,29 +3723,29 @@
       <c r="BR24" s="23"/>
       <c r="BS24" s="23"/>
     </row>
-    <row r="25" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="25" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
-      <c r="B25" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="63">
-        <v>0.6</v>
-      </c>
-      <c r="E25" s="54">
-        <f ca="1">E22+7</f>
+      <c r="B25" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="60">
+        <v>1</v>
+      </c>
+      <c r="E25" s="51">
+        <f>E22+7</f>
         <v>44704</v>
       </c>
-      <c r="F25" s="54">
-        <f ca="1">E25+6</f>
-        <v>44710</v>
+      <c r="F25" s="51">
+        <f>E25+4</f>
+        <v>44708</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="16">
-        <f t="shared" ca="1" si="12"/>
-        <v>7</v>
+        <f t="shared" si="12"/>
+        <v>5</v>
       </c>
       <c r="I25" s="23"/>
       <c r="J25" s="23"/>
@@ -3806,13 +3811,13 @@
       <c r="BR25" s="23"/>
       <c r="BS25" s="23"/>
     </row>
-    <row r="26" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="26" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
       <c r="I26" s="23"/>
@@ -3879,29 +3884,29 @@
       <c r="BR26" s="23"/>
       <c r="BS26" s="23"/>
     </row>
-    <row r="27" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="27" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37"/>
-      <c r="B27" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="53">
-        <v>0</v>
-      </c>
-      <c r="E27" s="54">
-        <f ca="1">E24+7</f>
+      <c r="B27" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="50">
+        <v>1</v>
+      </c>
+      <c r="E27" s="51">
+        <f>E24+7</f>
         <v>44711</v>
       </c>
-      <c r="F27" s="54">
-        <f ca="1">E27+13</f>
-        <v>44724</v>
+      <c r="F27" s="51">
+        <f>E27+10</f>
+        <v>44721</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="16">
-        <f t="shared" ca="1" si="12"/>
-        <v>14</v>
+        <f t="shared" si="12"/>
+        <v>11</v>
       </c>
       <c r="I27" s="23"/>
       <c r="J27" s="23"/>
@@ -3967,28 +3972,28 @@
       <c r="BR27" s="23"/>
       <c r="BS27" s="23"/>
     </row>
-    <row r="28" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="28" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
-      <c r="B28" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="53">
-        <v>0</v>
-      </c>
-      <c r="E28" s="54">
-        <f ca="1">E25+10</f>
+      <c r="B28" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="50">
+        <v>1</v>
+      </c>
+      <c r="E28" s="51">
+        <f>E25+10</f>
         <v>44714</v>
       </c>
-      <c r="F28" s="54">
-        <f ca="1">E28+7</f>
+      <c r="F28" s="51">
+        <f>E28+7</f>
         <v>44721</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="16">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="I28" s="23"/>
@@ -4055,28 +4060,28 @@
       <c r="BR28" s="23"/>
       <c r="BS28" s="23"/>
     </row>
-    <row r="29" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="29" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="37"/>
-      <c r="B29" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="53">
-        <v>0</v>
-      </c>
-      <c r="E29" s="54">
-        <f ca="1">E27+7</f>
+      <c r="B29" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="50">
+        <v>1</v>
+      </c>
+      <c r="E29" s="51">
+        <f>E27+7</f>
         <v>44718</v>
       </c>
-      <c r="F29" s="54">
-        <f t="shared" ref="F29:F31" ca="1" si="13">E29+6</f>
+      <c r="F29" s="51">
+        <f>E29+6</f>
         <v>44724</v>
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="16">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="I29" s="23"/>
@@ -4143,13 +4148,13 @@
       <c r="BR29" s="23"/>
       <c r="BS29" s="23"/>
     </row>
-    <row r="30" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="30" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="37"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
       <c r="I30" s="23"/>
@@ -4216,29 +4221,29 @@
       <c r="BR30" s="23"/>
       <c r="BS30" s="23"/>
     </row>
-    <row r="31" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="31" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
-      <c r="B31" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31" s="53">
-        <v>0</v>
-      </c>
-      <c r="E31" s="54">
-        <f ca="1">E27+7</f>
-        <v>44718</v>
-      </c>
-      <c r="F31" s="54">
-        <f ca="1">E31+7</f>
+      <c r="B31" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="50">
+        <v>1</v>
+      </c>
+      <c r="E31" s="51">
+        <f>E27+14</f>
         <v>44725</v>
+      </c>
+      <c r="F31" s="51">
+        <f>E31+9</f>
+        <v>44734</v>
       </c>
       <c r="G31" s="16"/>
       <c r="H31" s="16">
-        <f t="shared" ca="1" si="12"/>
-        <v>8</v>
+        <f t="shared" si="12"/>
+        <v>10</v>
       </c>
       <c r="I31" s="23"/>
       <c r="J31" s="23"/>
@@ -4304,12 +4309,12 @@
       <c r="BR31" s="23"/>
       <c r="BS31" s="23"/>
     </row>
-    <row r="32" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="32" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="38" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="19"/>
@@ -4317,7 +4322,7 @@
       <c r="F32" s="21"/>
       <c r="G32" s="22"/>
       <c r="H32" s="22" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I32" s="25"/>
@@ -4384,14 +4389,14 @@
       <c r="BR32" s="25"/>
       <c r="BS32" s="25"/>
     </row>
-    <row r="33" spans="3:7" ht="30" customHeight="1">
+    <row r="33" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="3:7" ht="30" customHeight="1">
+    <row r="34" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="14"/>
       <c r="F34" s="39"/>
     </row>
-    <row r="35" spans="3:7" ht="30" customHeight="1">
+    <row r="35" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="15"/>
     </row>
   </sheetData>
@@ -4489,7 +4494,7 @@
       <formula>AND(task_end&gt;=BM$5,task_start&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="E4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
@@ -4545,88 +4550,88 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="87.140625" style="27" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="87.109375" style="27" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1"/>
-    <row r="2" spans="1:2" s="29" customFormat="1" ht="15.75">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="28"/>
+    </row>
+    <row r="3" spans="1:2" s="33" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="34"/>
+    </row>
+    <row r="4" spans="1:2" s="30" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A4" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:2" s="33" customFormat="1" ht="27" customHeight="1">
-      <c r="A3" s="47" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="34"/>
-    </row>
-    <row r="4" spans="1:2" s="30" customFormat="1" ht="25.5">
-      <c r="A4" s="31" t="s">
+    </row>
+    <row r="7" spans="1:2" s="27" customFormat="1" ht="204.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1">
-      <c r="A5" s="32" t="s">
+    <row r="8" spans="1:2" s="30" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A8" s="31" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1">
-      <c r="A6" s="31" t="s">
+    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="27" customFormat="1" ht="204.95" customHeight="1">
-      <c r="A7" s="36" t="s">
+    <row r="10" spans="1:2" s="27" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="35" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="30" customFormat="1" ht="25.5">
-      <c r="A8" s="31" t="s">
+    <row r="11" spans="1:2" s="30" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A11" s="31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="42.75">
-      <c r="A9" s="32" t="s">
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="27" customFormat="1" ht="27.95" customHeight="1">
-      <c r="A10" s="35" t="s">
+    <row r="13" spans="1:2" s="27" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="35" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="30" customFormat="1" ht="25.5">
-      <c r="A11" s="31" t="s">
+    <row r="14" spans="1:2" s="30" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A14" s="31" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.5">
-      <c r="A12" s="32" t="s">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="27" customFormat="1" ht="27.95" customHeight="1">
-      <c r="A13" s="35" t="s">
+    <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="30" customFormat="1" ht="25.5">
-      <c r="A14" s="31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1">
-      <c r="A15" s="32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="57">
-      <c r="A16" s="32" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>